<commit_message>
updates to data inputs
</commit_message>
<xml_diff>
--- a/data-raw/sacwam_input.xlsx
+++ b/data-raw/sacwam_input.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/mwd-interoperable-flows/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A7DAFB2-D495-EC4C-B2C2-F7260EEEAAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579C58D1-305B-7243-9F32-EEB91613531E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="500" windowWidth="36440" windowHeight="19160" xr2:uid="{B1E2822F-1567-A442-A7A1-D098A8181CAB}"/>
+    <workbookView xWindow="28900" yWindow="3420" windowWidth="37400" windowHeight="26960" xr2:uid="{B1E2822F-1567-A442-A7A1-D098A8181CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="1" r:id="rId1"/>
     <sheet name="spatial_extent" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t xml:space="preserve">Data </t>
   </si>
@@ -111,9 +111,6 @@
     <t>Crop water demands</t>
   </si>
   <si>
-    <t>daily time step using dual crop coefficient approach described in FAO Drainage Paper (Allen et al. 1998) - MABIA method. Requires inputs of temperature, precipitation, humidity, wind speed. These inputs used to calculated a reference evapotranspiration using the Penman-Monteith Equation. Also requires soil parameters such as soil water capacity and soil depth. The Soil Conservation Service curve number method is used to calculate effective rainfall and rainfall-runoff. Crop use parameters based on the Sacramento - San Joaquin Basin Study (Reclamation, 2014C) - planting dates, season length, single crop coefficient</t>
-  </si>
-  <si>
     <t>Climate</t>
   </si>
   <si>
@@ -244,6 +241,30 @@
   </si>
   <si>
     <t>Reclamation'c CVP Contractor data</t>
+  </si>
+  <si>
+    <t>Land cover</t>
+  </si>
+  <si>
+    <t>National Land Cover Database 2011</t>
+  </si>
+  <si>
+    <t>Timestep</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daily time step using dual crop coefficient approach described in FAO Drainage Paper (Allen et al. 1998) - MABIA method. Requires inputs of temperature, precipitation, humidity, wind speed. These inputs used to calculated a reference evapotranspiration using the Penman-Monteith Equation. Also requires soil parameters such as soil water capacity and soil depth. The Soil Conservation Service curve number method is used to calculate effective rainfall and rainfall-runoff. </t>
+  </si>
+  <si>
+    <t>FAO Drainage Paper (Allen et al. 1998) - MABIA method; Crop use parameters based on the Sacramento - San Joaquin Basin Study (Reclamation, 2014C) - planting dates, season length, single crop coefficient</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Demand</t>
   </si>
 </sst>
 </file>
@@ -287,9 +308,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,195 +628,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB487E6E-2A5A-2043-B6DC-7E6DDE31BA3C}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
         <v>68</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -815,321 +901,321 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
         <v>59</v>
       </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>